<commit_message>
add read me file
</commit_message>
<xml_diff>
--- a/excel/BookingTestData.xlsx
+++ b/excel/BookingTestData.xlsx
@@ -421,10 +421,10 @@
         <v>Alexandria</v>
       </c>
       <c r="B2" t="str">
-        <v>2025-11-02</v>
+        <v>2025-11-25</v>
       </c>
       <c r="C2" t="str">
-        <v>2026-01-01</v>
+        <v>2026-01-24</v>
       </c>
       <c r="D2" t="str">
         <v>Tolip Hotel Alexandria</v>

</xml_diff>